<commit_message>
code changes for scheduling based test cases
</commit_message>
<xml_diff>
--- a/TestData/AmortTemplateTelemundo.xlsx
+++ b/TestData/AmortTemplateTelemundo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="7215" tabRatio="643"/>
   </bookViews>
   <sheets>
     <sheet name="AmortTemplateGrid" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="50">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,154 +566,40 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>191</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>206</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2997,8 +2883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>